<commit_message>
Fixes Industrial sector scaling map
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/Argentina_scaling_mapping.xlsx
+++ b/input/mappings/scaling/Argentina_scaling_mapping.xlsx
@@ -11,7 +11,7 @@
     <sheet name="year" sheetId="2" r:id="rId2"/>
     <sheet name="method" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="111">
   <si>
     <t>Energy</t>
   </si>
@@ -452,8 +452,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="101">
+  <cellStyleXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -570,7 +572,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="101">
+  <cellStyles count="103">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -621,6 +623,7 @@
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -671,6 +674,7 @@
     <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -941,7 +945,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -952,7 +956,7 @@
   <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:B24"/>
+      <selection activeCell="B24" sqref="B24:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1178,12 +1182,17 @@
         <v>55</v>
       </c>
     </row>
+    <row r="25" spans="1:3">
+      <c r="B25" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="26" spans="1:3">
       <c r="A26" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="C26" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:3">

</xml_diff>

<commit_message>
Updates to mapping files. (Remove shipping and aviation, other changes.)
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/Argentina_scaling_mapping.xlsx
+++ b/input/mappings/scaling/Argentina_scaling_mapping.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="111">
   <si>
     <t>Energy</t>
   </si>
@@ -955,8 +955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="E88" sqref="E88"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1204,9 +1204,6 @@
       <c r="A28" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B28" t="s">
-        <v>101</v>
-      </c>
       <c r="C28" t="s">
         <v>101</v>
       </c>
@@ -1218,9 +1215,6 @@
       <c r="A30" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B30" t="s">
-        <v>57</v>
-      </c>
       <c r="C30" t="s">
         <v>57</v>
       </c>
@@ -1268,9 +1262,6 @@
       <c r="A38" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B38" t="s">
-        <v>60</v>
-      </c>
       <c r="C38" t="s">
         <v>60</v>
       </c>
@@ -1278,9 +1269,6 @@
     <row r="39" spans="1:3">
       <c r="A39" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="B39" t="s">
-        <v>100</v>
       </c>
       <c r="C39" t="s">
         <v>100</v>

</xml_diff>